<commit_message>
Added missing widths, refractive index refrence and example bibliography
</commit_message>
<xml_diff>
--- a/Molecular Spectroscopy/Analysis/Summary.xlsx
+++ b/Molecular Spectroscopy/Analysis/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alon4\Dropbox\Labs\Lab C1\Molecular Spectroscopy\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924BA405-AD06-4799-928E-D7400BF4B4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861A295-C735-4974-AFCD-5CFD51E6D6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Marlbro</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Isoprene</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F22"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -764,25 +767,50 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <f>SUM(B14:B21)</f>
+        <v>99.870540870497422</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:F22" si="10">SUM(C14:C21)</f>
+        <v>58.730653877023151</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="10"/>
+        <v>72.797915830813253</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="10"/>
+        <v>72.797915830813253</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="10"/>
+        <v>99.976331324490872</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="3"/>
+      <c r="B23">
+        <f>B11/B$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="3"/>
+      <c r="C23">
+        <f>C11/C$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
+      <c r="D23">
+        <f>D11/D$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
+      <c r="E23">
+        <f>E11/E$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <f>F11/F$11%</f>
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Added substance tables, and wrote about results
</commit_message>
<xml_diff>
--- a/Molecular Spectroscopy/Analysis/Summary.xlsx
+++ b/Molecular Spectroscopy/Analysis/Summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alon4\Dropbox\Labs\Lab C1\Molecular Spectroscopy\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alon4\Dropbox\My PC (LAPTOP-L5MMEHHN)\Desktop\Studies\Lab C1\Molecular Spectroscopy\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D861A295-C735-4974-AFCD-5CFD51E6D6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051156F7-D941-4396-AAB5-B5EB77FEBA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8556" yWindow="888" windowWidth="14484" windowHeight="8448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,153 +396,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>17.639399999999998</v>
+      </c>
+      <c r="C2">
+        <v>6.5842000000000001</v>
+      </c>
+      <c r="D2">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="E2">
+        <v>21.938800000000001</v>
+      </c>
+      <c r="F2">
+        <v>21.938800000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>177.08670000000001</v>
       </c>
       <c r="C3">
-        <v>3.0964999999999998</v>
+        <v>69.248800000000003</v>
       </c>
       <c r="D3">
-        <v>3.1671999999999998</v>
+        <v>174.36799999999999</v>
       </c>
       <c r="E3">
-        <v>3.1671999999999998</v>
+        <v>239.13579999999999</v>
+      </c>
+      <c r="F3">
+        <v>239.13579999999999</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.36980000000000002</v>
-      </c>
-      <c r="D4">
-        <v>0.51129999999999998</v>
       </c>
       <c r="E4">
         <v>0.51129999999999998</v>
       </c>
+      <c r="F4">
+        <v>0.51129999999999998</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>0.27879999999999999</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>0.35270000000000001</v>
+        <v>4.4847000000000001</v>
       </c>
       <c r="E5">
-        <v>0.35270000000000001</v>
+        <v>4.2874999999999996</v>
+      </c>
+      <c r="F5">
+        <v>4.2874999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>63.69</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>91.120400000000004</v>
+        <v>3.0964999999999998</v>
       </c>
       <c r="E6">
-        <v>91.120400000000004</v>
+        <v>3.1671999999999998</v>
+      </c>
+      <c r="F6">
+        <v>3.1671999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>4.4847000000000001</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>4.2874999999999996</v>
+        <v>0.27879999999999999</v>
       </c>
       <c r="E7">
-        <v>4.2874999999999996</v>
+        <v>0.35270000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.35270000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>43.165300000000002</v>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>51.368899999999996</v>
+        <v>63.69</v>
       </c>
       <c r="E8">
-        <v>51.368899999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>6.5842000000000001</v>
-      </c>
-      <c r="C9">
-        <v>17.809999999999999</v>
-      </c>
-      <c r="D9">
-        <v>21.938800000000001</v>
-      </c>
-      <c r="E9">
-        <v>21.938800000000001</v>
-      </c>
-      <c r="F9">
-        <v>17.639399999999998</v>
+        <v>91.120400000000004</v>
+      </c>
+      <c r="F8">
+        <v>91.120400000000004</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>69.248800000000003</v>
-      </c>
-      <c r="C10">
-        <v>174.36799999999999</v>
+        <v>9</v>
       </c>
       <c r="D10">
-        <v>239.13579999999999</v>
+        <v>43.165300000000002</v>
       </c>
       <c r="E10">
-        <v>239.13579999999999</v>
+        <v>51.368899999999996</v>
       </c>
       <c r="F10">
-        <v>177.08670000000001</v>
+        <v>51.368899999999996</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -550,19 +550,19 @@
         <v>12</v>
       </c>
       <c r="B11">
+        <v>194.7722</v>
+      </c>
+      <c r="C11">
         <v>75.931299999999993</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>523.17330000000004</v>
-      </c>
-      <c r="D11">
-        <v>565.78899999999999</v>
       </c>
       <c r="E11">
         <v>565.78899999999999</v>
       </c>
       <c r="F11">
-        <v>194.7722</v>
+        <v>565.78899999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,23 +570,23 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14" si="0">B3/B$11 * 100</f>
+        <f>C6/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C14">
-        <f>C3/C$11 * 100</f>
+        <f>D6/D$11 * 100</f>
         <v>0.59186888933361081</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:F14" si="1">D3/D$11 * 100</f>
+        <f>E6/E$11 * 100</f>
         <v>0.55978465470343186</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f>F6/F$11 * 100</f>
         <v>0.55978465470343186</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f>B6/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -595,23 +595,23 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15" si="2">B4/B$11 * 100</f>
+        <f>C4/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="B15:F22" si="3">C4/C$11 * 100</f>
+        <f>D4/D$11 * 100</f>
         <v>7.0684035290027217E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f>E4/E$11 * 100</f>
         <v>9.0369377983665289E-2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
+        <f>F4/F$11 * 100</f>
         <v>9.0369377983665289E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f>B4/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -620,23 +620,23 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16" si="4">B5/B$11 * 100</f>
+        <f>C7/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f>D7/D$11 * 100</f>
         <v>5.3290181284098397E-2</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f>E7/E$11 * 100</f>
         <v>6.2337726608329258E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f>F7/F$11 * 100</f>
         <v>6.2337726608329258E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f>B7/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -645,23 +645,23 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17" si="5">B6/B$11 * 100</f>
+        <f>C8/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="3"/>
+        <f>D8/D$11 * 100</f>
         <v>12.173786391622048</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f>E8/E$11 * 100</f>
         <v>16.105014413500442</v>
       </c>
       <c r="E17">
-        <f t="shared" si="3"/>
+        <f>F8/F$11 * 100</f>
         <v>16.105014413500442</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f>B8/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -670,23 +670,23 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18" si="6">B7/B$11 * 100</f>
+        <f>C5/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C18">
-        <f t="shared" si="3"/>
+        <f>D5/D$11 * 100</f>
         <v>0.85721117648779099</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f>E5/E$11 * 100</f>
         <v>0.757791332104371</v>
       </c>
       <c r="E18">
-        <f t="shared" si="3"/>
+        <f>F5/F$11 * 100</f>
         <v>0.757791332104371</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f>B5/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -695,23 +695,23 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19" si="7">B8/B$11 * 100</f>
+        <f>C10/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C19">
-        <f t="shared" si="3"/>
+        <f>D10/D$11 * 100</f>
         <v>8.2506695200232887</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f>E10/E$11 * 100</f>
         <v>9.079162019763551</v>
       </c>
       <c r="E19">
-        <f t="shared" si="3"/>
+        <f>F10/F$11 * 100</f>
         <v>9.079162019763551</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f>B10/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
@@ -720,23 +720,23 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20" si="8">B9/B$11 * 100</f>
+        <f>C2/C$11 * 100</f>
         <v>8.6712594147604491</v>
       </c>
       <c r="C20">
-        <f t="shared" si="3"/>
+        <f>D2/D$11 * 100</f>
         <v>3.4042257125889255</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f>E2/E$11 * 100</f>
         <v>3.8775585951653353</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f>F2/F$11 * 100</f>
         <v>3.8775585951653353</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f>B2/B$11 * 100</f>
         <v>9.0564259170456562</v>
       </c>
     </row>
@@ -745,23 +745,23 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21" si="9">B10/B$11 * 100</f>
+        <f>C3/C$11 * 100</f>
         <v>91.199281455736966</v>
       </c>
       <c r="C21">
-        <f t="shared" si="3"/>
+        <f>D3/D$11 * 100</f>
         <v>33.328917970393363</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f>E3/E$11 * 100</f>
         <v>42.265897710984127</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
+        <f>F3/F$11 * 100</f>
         <v>42.265897710984127</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f>B3/B$11 * 100</f>
         <v>90.919905407445214</v>
       </c>
     </row>
@@ -774,19 +774,19 @@
         <v>99.870540870497422</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:F22" si="10">SUM(C14:C21)</f>
+        <f t="shared" ref="C22:F22" si="0">SUM(C14:C21)</f>
         <v>58.730653877023151</v>
       </c>
       <c r="D22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>72.797915830813253</v>
       </c>
       <c r="E22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>72.797915830813253</v>
       </c>
       <c r="F22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>99.976331324490872</v>
       </c>
     </row>
@@ -795,23 +795,23 @@
         <v>12</v>
       </c>
       <c r="B23">
-        <f>B11/B$11 * 100</f>
-        <v>100</v>
-      </c>
-      <c r="C23">
         <f>C11/C$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="D23">
+      <c r="C23">
         <f>D11/D$11 * 100</f>
         <v>100</v>
       </c>
-      <c r="E23">
+      <c r="D23">
         <f>E11/E$11 * 100</f>
         <v>100</v>
       </c>
+      <c r="E23">
+        <f>F11/F$11 * 100</f>
+        <v>100</v>
+      </c>
       <c r="F23">
-        <f>F11/F$11%</f>
+        <f>B11/B$11%</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed cigar tables in results
</commit_message>
<xml_diff>
--- a/Molecular Spectroscopy/Analysis/Summary.xlsx
+++ b/Molecular Spectroscopy/Analysis/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alon4\Dropbox\My PC (LAPTOP-L5MMEHHN)\Desktop\Studies\Lab C1\Molecular Spectroscopy\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051156F7-D941-4396-AAB5-B5EB77FEBA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F949973A-E20D-41B0-B5E9-806185F6E993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8556" yWindow="888" windowWidth="14484" windowHeight="8448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Marlbro</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>LM00</t>
   </si>
 </sst>
 </file>
@@ -396,32 +399,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -432,16 +438,19 @@
         <v>6.5842000000000001</v>
       </c>
       <c r="D2">
+        <v>12.166</v>
+      </c>
+      <c r="E2">
         <v>17.809999999999999</v>
-      </c>
-      <c r="E2">
-        <v>21.938800000000001</v>
       </c>
       <c r="F2">
         <v>21.938800000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>21.938800000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -452,100 +461,103 @@
         <v>69.248800000000003</v>
       </c>
       <c r="D3">
+        <v>144.9974</v>
+      </c>
+      <c r="E3">
         <v>174.36799999999999</v>
-      </c>
-      <c r="E3">
-        <v>239.13579999999999</v>
       </c>
       <c r="F3">
         <v>239.13579999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>239.13579999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.36980000000000002</v>
-      </c>
-      <c r="E4">
-        <v>0.51129999999999998</v>
       </c>
       <c r="F4">
         <v>0.51129999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.51129999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4.4847000000000001</v>
-      </c>
-      <c r="E5">
-        <v>4.2874999999999996</v>
       </c>
       <c r="F5">
         <v>4.2874999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>4.2874999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3.0964999999999998</v>
-      </c>
-      <c r="E6">
-        <v>3.1671999999999998</v>
       </c>
       <c r="F6">
         <v>3.1671999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>3.1671999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.27879999999999999</v>
-      </c>
-      <c r="E7">
-        <v>0.35270000000000001</v>
       </c>
       <c r="F7">
         <v>0.35270000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0.35270000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>63.69</v>
-      </c>
-      <c r="E8">
-        <v>91.120400000000004</v>
       </c>
       <c r="F8">
         <v>91.120400000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>91.120400000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>43.165300000000002</v>
-      </c>
-      <c r="E10">
-        <v>51.368899999999996</v>
       </c>
       <c r="F10">
         <v>51.368899999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>51.368899999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -555,17 +567,17 @@
       <c r="C11">
         <v>75.931299999999993</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>523.17330000000004</v>
-      </c>
-      <c r="E11">
-        <v>565.78899999999999</v>
       </c>
       <c r="F11">
         <v>565.78899999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>565.78899999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -574,23 +586,23 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <f>D6/D$11 * 100</f>
+        <f>E6/E$11 * 100</f>
         <v>0.59186888933361081</v>
-      </c>
-      <c r="D14">
-        <f>E6/E$11 * 100</f>
-        <v>0.55978465470343186</v>
       </c>
       <c r="E14">
         <f>F6/F$11 * 100</f>
         <v>0.55978465470343186</v>
       </c>
       <c r="F14">
+        <f>G6/G$11 * 100</f>
+        <v>0.55978465470343186</v>
+      </c>
+      <c r="G14">
         <f>B6/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -599,73 +611,73 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <f>D4/D$11 * 100</f>
+        <f>E4/E$11 * 100</f>
         <v>7.0684035290027217E-2</v>
-      </c>
-      <c r="D15">
-        <f>E4/E$11 * 100</f>
-        <v>9.0369377983665289E-2</v>
       </c>
       <c r="E15">
         <f>F4/F$11 * 100</f>
         <v>9.0369377983665289E-2</v>
       </c>
       <c r="F15">
+        <f>G4/G$11 * 100</f>
+        <v>9.0369377983665289E-2</v>
+      </c>
+      <c r="G15">
         <f>B4/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16">
-        <f>C7/C$11 * 100</f>
+        <f t="shared" ref="B16:B17" si="0">C7/C$11 * 100</f>
         <v>0</v>
       </c>
       <c r="C16">
-        <f>D7/D$11 * 100</f>
+        <f>E7/E$11 * 100</f>
         <v>5.3290181284098397E-2</v>
-      </c>
-      <c r="D16">
-        <f>E7/E$11 * 100</f>
-        <v>6.2337726608329258E-2</v>
       </c>
       <c r="E16">
         <f>F7/F$11 * 100</f>
         <v>6.2337726608329258E-2</v>
       </c>
       <c r="F16">
+        <f>G7/G$11 * 100</f>
+        <v>6.2337726608329258E-2</v>
+      </c>
+      <c r="G16">
         <f>B7/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17">
-        <f>C8/C$11 * 100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C17">
-        <f>D8/D$11 * 100</f>
+        <f>E8/E$11 * 100</f>
         <v>12.173786391622048</v>
-      </c>
-      <c r="D17">
-        <f>E8/E$11 * 100</f>
-        <v>16.105014413500442</v>
       </c>
       <c r="E17">
         <f>F8/F$11 * 100</f>
         <v>16.105014413500442</v>
       </c>
       <c r="F17">
+        <f>G8/G$11 * 100</f>
+        <v>16.105014413500442</v>
+      </c>
+      <c r="G17">
         <f>B8/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -674,23 +686,23 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <f>D5/D$11 * 100</f>
+        <f>E5/E$11 * 100</f>
         <v>0.85721117648779099</v>
-      </c>
-      <c r="D18">
-        <f>E5/E$11 * 100</f>
-        <v>0.757791332104371</v>
       </c>
       <c r="E18">
         <f>F5/F$11 * 100</f>
         <v>0.757791332104371</v>
       </c>
       <c r="F18">
+        <f>G5/G$11 * 100</f>
+        <v>0.757791332104371</v>
+      </c>
+      <c r="G18">
         <f>B5/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -699,73 +711,73 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <f>D10/D$11 * 100</f>
+        <f>E10/E$11 * 100</f>
         <v>8.2506695200232887</v>
-      </c>
-      <c r="D19">
-        <f>E10/E$11 * 100</f>
-        <v>9.079162019763551</v>
       </c>
       <c r="E19">
         <f>F10/F$11 * 100</f>
         <v>9.079162019763551</v>
       </c>
       <c r="F19">
+        <f>G10/G$11 * 100</f>
+        <v>9.079162019763551</v>
+      </c>
+      <c r="G19">
         <f>B10/B$11 * 100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
       <c r="B20">
-        <f>C2/C$11 * 100</f>
+        <f t="shared" ref="B20:B21" si="1">C2/C$11 * 100</f>
         <v>8.6712594147604491</v>
       </c>
       <c r="C20">
-        <f>D2/D$11 * 100</f>
+        <f>E2/E$11 * 100</f>
         <v>3.4042257125889255</v>
-      </c>
-      <c r="D20">
-        <f>E2/E$11 * 100</f>
-        <v>3.8775585951653353</v>
       </c>
       <c r="E20">
         <f>F2/F$11 * 100</f>
         <v>3.8775585951653353</v>
       </c>
       <c r="F20">
+        <f>G2/G$11 * 100</f>
+        <v>3.8775585951653353</v>
+      </c>
+      <c r="G20">
         <f>B2/B$11 * 100</f>
         <v>9.0564259170456562</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
       <c r="B21">
-        <f>C3/C$11 * 100</f>
+        <f t="shared" si="1"/>
         <v>91.199281455736966</v>
       </c>
       <c r="C21">
-        <f>D3/D$11 * 100</f>
+        <f>E3/E$11 * 100</f>
         <v>33.328917970393363</v>
-      </c>
-      <c r="D21">
-        <f>E3/E$11 * 100</f>
-        <v>42.265897710984127</v>
       </c>
       <c r="E21">
         <f>F3/F$11 * 100</f>
         <v>42.265897710984127</v>
       </c>
       <c r="F21">
+        <f>G3/G$11 * 100</f>
+        <v>42.265897710984127</v>
+      </c>
+      <c r="G21">
         <f>B3/B$11 * 100</f>
         <v>90.919905407445214</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -774,23 +786,23 @@
         <v>99.870540870497422</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:F22" si="0">SUM(C14:C21)</f>
+        <f t="shared" ref="C22" si="2">SUM(C14:C21)</f>
         <v>58.730653877023151</v>
       </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
+      <c r="E22">
+        <f>SUM(E14:E21)</f>
         <v>72.797915830813253</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="F22">
+        <f>SUM(F14:F21)</f>
         <v>72.797915830813253</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
+      <c r="G22">
+        <f>SUM(G14:G21)</f>
         <v>99.976331324490872</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -799,10 +811,6 @@
         <v>100</v>
       </c>
       <c r="C23">
-        <f>D11/D$11 * 100</f>
-        <v>100</v>
-      </c>
-      <c r="D23">
         <f>E11/E$11 * 100</f>
         <v>100</v>
       </c>
@@ -811,6 +819,10 @@
         <v>100</v>
       </c>
       <c r="F23">
+        <f>G11/G$11 * 100</f>
+        <v>100</v>
+      </c>
+      <c r="G23">
         <f>B11/B$11%</f>
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
added LM cigar calculations in excel
</commit_message>
<xml_diff>
--- a/Molecular Spectroscopy/Analysis/Summary.xlsx
+++ b/Molecular Spectroscopy/Analysis/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alon4\Dropbox\My PC (LAPTOP-L5MMEHHN)\Desktop\Studies\Lab C1\Molecular Spectroscopy\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F949973A-E20D-41B0-B5E9-806185F6E993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F943B3-3157-4B26-BDE5-E94F3690CE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4812" yWindow="2028" windowWidth="14484" windowHeight="8448" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Marlbro</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>LM00</t>
+  </si>
+  <si>
+    <t>LM/LM00</t>
+  </si>
+  <si>
+    <t>ratio co2</t>
+  </si>
+  <si>
+    <t>concen co2</t>
+  </si>
+  <si>
+    <t>next</t>
   </si>
 </sst>
 </file>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -827,6 +839,56 @@
         <v>100</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <f>D2/E2</f>
+        <v>0.68309938236945544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <f>D3/E3</f>
+        <v>0.83155968985134887</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <f>100*B28</f>
+        <v>83.155968985134891</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <f>4.1*B28</f>
+        <v>3.4093947283905299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31">
+        <f>B27*1.2</f>
+        <v>0.81971925884334651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>